<commit_message>
Update formating on Excel and CSV files.
</commit_message>
<xml_diff>
--- a/2016_Income_Data.xlsx
+++ b/2016_Income_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yamellmejia/Desktop/UM Data Analytics BootCamp/Projects/Project 1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dalto\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3BE04771-CEC8-244B-99FA-D24B0F4CA6C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D9A7736-6EAC-4275-BD74-820DC173C865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{FF8A7A06-A228-41D3-9463-98779EA21889}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FF8A7A06-A228-41D3-9463-98779EA21889}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -148,7 +148,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor rgb="FF36AF63"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -238,7 +238,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -250,15 +250,11 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -610,189 +606,189 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection sqref="A1:E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.1640625" customWidth="1"/>
+    <col min="1" max="1" width="33.109375" customWidth="1"/>
     <col min="2" max="2" width="34" customWidth="1"/>
-    <col min="3" max="3" width="31.1640625" customWidth="1"/>
-    <col min="4" max="4" width="23.5" customWidth="1"/>
-    <col min="5" max="5" width="26.83203125" customWidth="1"/>
+    <col min="3" max="3" width="31.109375" customWidth="1"/>
+    <col min="4" max="4" width="23.44140625" customWidth="1"/>
+    <col min="5" max="5" width="26.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:5" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="1">
         <v>87057</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="1">
         <v>695</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="1">
         <v>60804</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="1">
         <v>41027</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="1">
         <v>871</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="1">
         <v>15572</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="1">
         <v>58051</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="1">
         <v>2172</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="1">
         <v>6452</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="1">
         <v>30572</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="1">
         <v>603</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="1">
         <v>22858</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="1">
         <v>41749</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="1">
         <v>701</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="1">
         <v>20539</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="1">
         <v>61858</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="1">
         <v>549</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="1">
         <v>99400</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="1">
         <v>39490</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="1">
         <v>1187</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="1">
         <v>16733</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="1">
         <v>81431</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="1">
         <v>1917</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="1">
         <v>6392</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="1">
         <v>47675</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="1">
         <v>1113</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="1">
         <v>16915</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>5</v>
       </c>
@@ -809,7 +805,7 @@
         <v>6238</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>5</v>
       </c>
@@ -826,7 +822,7 @@
         <v>20109</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>5</v>
       </c>
@@ -843,7 +839,7 @@
         <v>21500</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>5</v>
       </c>
@@ -860,7 +856,7 @@
         <v>22808</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>5</v>
       </c>
@@ -877,7 +873,7 @@
         <v>23770</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>5</v>
       </c>

</xml_diff>